<commit_message>
3D histogram visualisation of data
</commit_message>
<xml_diff>
--- a/results/simulation-results.xlsx
+++ b/results/simulation-results.xlsx
@@ -5,26 +5,26 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajaamour/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajaamour/Projects/ICCS-2/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6612FAA5-5B3F-1C45-ACB2-A71522DD2298}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2B8A84-29BE-6D47-AD06-8E8AF6946B8E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19180" yWindow="460" windowWidth="14420" windowHeight="19060" xr2:uid="{B3C17F0F-8055-454C-AB13-ED0A7235AE55}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="150001"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -100,9 +100,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -138,16 +135,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -155,29 +152,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCE835B"/>
+      <color rgb="FFF49854"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -187,6 +193,1389 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="230"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.0232222222222238E-2"/>
+          <c:y val="2.7718253968253968E-2"/>
+          <c:w val="0.86813740740740741"/>
+          <c:h val="0.91438194444444443"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.001</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:shade val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000010-024B-6347-A879-B3218C0BB546}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-6713-514F-9292-83E6614E6067}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="CE835B"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-6713-514F-9292-83E6614E6067}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$F$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$6:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>501</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>749</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-6713-514F-9292-83E6614E6067}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-6713-514F-9292-83E6614E6067}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-6713-514F-9292-83E6614E6067}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="CE835B"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-6713-514F-9292-83E6614E6067}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$F$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$7:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>431</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>716</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-6713-514F-9292-83E6614E6067}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-6713-514F-9292-83E6614E6067}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-6713-514F-9292-83E6614E6067}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$F$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$8:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>549</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000012-6713-514F-9292-83E6614E6067}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="0"/>
+        <c:gapDepth val="0"/>
+        <c:shape val="box"/>
+        <c:axId val="1911636800"/>
+        <c:axId val="1911637328"/>
+        <c:axId val="1921652656"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="1911636800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="2400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Cost of</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Living</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.16362314814814816"/>
+              <c:y val="0.78707777777777788"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="2400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1911637328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1911637328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Ticks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.93909759259259262"/>
+              <c:y val="0.42154801587301588"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1911636800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="1921652656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-1740000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Suicide Rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.67576629629629636"/>
+              <c:y val="0.81963154761904755"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-1740000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1911637328"/>
+        <c:crosses val="autoZero"/>
+      </c:serAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
+  <a:schemeClr val="accent1"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="307">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -209,7 +1598,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB22C7EF-406A-D343-92D6-17741A5565B6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -253,7 +1642,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB0BEC5D-AB71-EB43-B4B0-E751C7BE32C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -297,7 +1686,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6731E662-5605-4549-B345-00F2F03CD3DB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -341,7 +1730,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E505A795-F62B-6E40-8302-56BAA3298DAF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -385,7 +1774,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F3684E6-D9C8-484A-9656-6ED9F74DB437}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -429,7 +1818,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31B26888-E173-2849-B7CF-C4B9486C5934}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -473,7 +1862,7 @@
         <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17C08C74-8981-3B49-9977-98E9BEA9C2F3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -517,7 +1906,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F83DF79-92EB-1D4F-B2AC-F6A3623C358B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -561,7 +1950,7 @@
         <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DB024CE-0A48-984B-A5AB-26A2AD7385AC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -605,7 +1994,7 @@
         <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51675352-CEF9-6D46-9308-3FF03AC07F7B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -649,7 +2038,7 @@
         <xdr:cNvPr id="12" name="Picture 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{924AD1E9-6D72-4246-B440-7A335B479DA0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -693,7 +2082,7 @@
         <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF23F303-52A4-0442-A08C-DC7BF33CCE95}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -737,7 +2126,7 @@
         <xdr:cNvPr id="14" name="Picture 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98E178C4-911B-0B47-86A0-2FFC52CA3B01}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -781,7 +2170,7 @@
         <xdr:cNvPr id="16" name="Picture 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AF61A32-6868-4A4B-93FE-8DF59283A20E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -805,6 +2194,42 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1592385</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>205153</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>368846</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>116307</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="Chart 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1106,11 +2531,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3750FAAB-82B9-E74C-91D1-79FE66587074}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:T37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1122,42 +2547,42 @@
   <sheetData>
     <row r="1" spans="2:20" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="2">
         <v>100</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="2">
         <v>0.5</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2" t="s">
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="2"/>
+      <c r="M3" s="1"/>
       <c r="P3" t="s">
         <v>13</v>
       </c>
@@ -1166,13 +2591,13 @@
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="2">
         <v>4900</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="4"/>
       <c r="F4">
         <v>0</v>
       </c>
@@ -1187,13 +2612,13 @@
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>2</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="3">
         <v>1E-4</v>
       </c>
       <c r="F5">
@@ -1269,27 +2694,27 @@
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="E14" s="3"/>
+      <c r="E14" s="7"/>
       <c r="F14">
         <v>0</v>
       </c>
@@ -1304,30 +2729,30 @@
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="E15" s="6">
+      <c r="E15" s="3">
         <v>1E-4</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="8">
         <v>0.37795918367346898</v>
       </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.2">
       <c r="E16">
         <v>1E-3</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="8">
         <v>0.49510204081632597</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="8">
         <v>0.41551020408163197</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="8">
         <v>0.54367346938775496</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="8">
         <v>0.50693877551020405</v>
       </c>
       <c r="L16" t="s">
@@ -1344,16 +2769,16 @@
       <c r="E17">
         <v>0.01</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="8">
         <v>0.56938775510203998</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="8">
         <v>0.65142857142857102</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="8">
         <v>0.47163265306122398</v>
       </c>
-      <c r="I17" s="7" t="s">
+      <c r="I17" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1361,16 +2786,16 @@
       <c r="E18">
         <v>0.1</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="8">
         <v>0.88734693877550996</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="8">
         <v>0.93142857142857105</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="8">
         <v>0.87306122448979595</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="I18" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1378,16 +2803,16 @@
       <c r="E19">
         <v>0.9</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="8">
         <v>0.96040816326530598</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="8">
         <v>0.98102040816326497</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="8">
         <v>0.94938775510203999</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="I19" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1395,7 +2820,7 @@
       <c r="L23" t="s">
         <v>9</v>
       </c>
-      <c r="O23" s="2" t="s">
+      <c r="O23" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1410,7 +2835,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="12:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C36" s="4"/>
+    </row>
+    <row r="37" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C37" s="3"/>
       <c r="L37" t="s">
         <v>18</v>
       </c>
@@ -1422,12 +2851,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="F13:I13"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="E12:I12"/>
-    <mergeCell ref="E3:E4"/>
     <mergeCell ref="E13:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>